<commit_message>
Added name to student excel
</commit_message>
<xml_diff>
--- a/student_list.xlsx
+++ b/student_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sarfaraz\maktab\Kalewadi\git-repo\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6D06E4-5707-4216-B1EF-E113EA7BCA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973CF55A-C799-4916-932E-2D0CC7ED75DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <t>Names</t>
   </si>
   <si>
-    <t>ADIBA AYAZ SAYYED Result</t>
+    <t>ADIBA AYAZ SAYYED RESULT</t>
   </si>
 </sst>
 </file>
@@ -184,7 +184,247 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="43">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -197,294 +437,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -515,227 +467,227 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1014,7 +966,7 @@
   <dimension ref="A1:D156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1654,135 +1606,123 @@
       <c r="D156" s="10"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D2:D145">
+    <cfRule type="duplicateValues" dxfId="42" priority="2034"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D146">
-    <cfRule type="expression" dxfId="46" priority="109">
+    <cfRule type="expression" dxfId="41" priority="109">
       <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="110">
+    <cfRule type="expression" dxfId="40" priority="110">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;#REF!&amp;#REF!))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="111">
+    <cfRule type="expression" dxfId="39" priority="111">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;#REF!&amp;#REF!))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="112">
-      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;$C148&amp;$D89))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="113">
-      <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C148&amp;$D89))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="114">
-      <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C147&amp;$D89))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D146:D155">
-    <cfRule type="expression" dxfId="40" priority="93">
+    <cfRule type="expression" dxfId="38" priority="93">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C143&amp;$D89))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="94">
+    <cfRule type="expression" dxfId="37" priority="94">
       <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;$C143&amp;$D89))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="95">
+    <cfRule type="expression" dxfId="36" priority="95">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C147&amp;$H143))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="96">
+    <cfRule type="expression" dxfId="35" priority="96">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;#REF!&amp;#REF!))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="97">
+    <cfRule type="expression" dxfId="34" priority="97">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;#REF!&amp;#REF!))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="98">
+    <cfRule type="expression" dxfId="33" priority="98">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C148&amp;$H143))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="99">
+    <cfRule type="expression" dxfId="32" priority="99">
       <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;$C148&amp;$H143))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="100">
+    <cfRule type="expression" dxfId="31" priority="100">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;#REF!&amp;#REF!))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="104">
+    <cfRule type="expression" dxfId="30" priority="104">
       <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="106">
+    <cfRule type="expression" dxfId="29" priority="106">
       <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="107">
+    <cfRule type="expression" dxfId="28" priority="107">
       <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="108">
+    <cfRule type="expression" dxfId="27" priority="108">
       <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="112">
+      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;$C148&amp;$D89))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="113">
+      <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C148&amp;$D89))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="114">
+      <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C147&amp;$D89))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D146:D156">
-    <cfRule type="duplicateValues" dxfId="28" priority="1946"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="2009"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="2014"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="2029"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="2014"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="1946"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="2009"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="2029"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147:D155">
-    <cfRule type="expression" dxfId="24" priority="131">
+    <cfRule type="expression" dxfId="19" priority="131">
       <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="132">
+    <cfRule type="expression" dxfId="18" priority="132">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;#REF!&amp;#REF!))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="133">
+    <cfRule type="expression" dxfId="17" priority="133">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;#REF!&amp;#REF!))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="134">
-      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;$C149&amp;$D90))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="135">
-      <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C149&amp;$D90))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="136">
-      <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C148&amp;$D90))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D156">
-    <cfRule type="expression" dxfId="18" priority="1980">
-      <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C153&amp;$D99))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="1981">
-      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;$C153&amp;$D99))</formula>
-    </cfRule>
     <cfRule type="expression" dxfId="16" priority="1982">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C157&amp;$H153))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="1983">
+    <cfRule type="expression" dxfId="15" priority="1984">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;#REF!&amp;#REF!))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="1984">
+    <cfRule type="expression" dxfId="14" priority="1985">
+      <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C158&amp;$H153))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="1986">
+      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;$C158&amp;$H153))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="1987">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;#REF!&amp;#REF!))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="1985">
-      <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C158&amp;$H153))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="1986">
-      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;$C158&amp;$H153))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="1987">
+    <cfRule type="expression" dxfId="11" priority="1991">
+      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="1993">
+      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="1994">
+      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="1996">
+      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="1997">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;#REF!&amp;#REF!))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="1991">
-      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="1993">
-      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="1994">
-      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="1995">
-      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="1996">
-      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="1997">
+    <cfRule type="expression" dxfId="6" priority="1980">
+      <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C153&amp;$D99))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="1983">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;#REF!&amp;#REF!))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="1998">
-      <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;#REF!&amp;#REF!))</formula>
+    <cfRule type="expression" dxfId="4" priority="1981">
+      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;$C153&amp;$D99))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="2031">
       <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;$C158&amp;$D99))</formula>
@@ -1793,9 +1733,9 @@
     <cfRule type="expression" dxfId="1" priority="2033">
       <formula>IF(ISBLANK($C$2),o,SEARCH($C$2,#REF!&amp;$C157&amp;$D99))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D145">
-    <cfRule type="duplicateValues" dxfId="0" priority="2034"/>
+    <cfRule type="expression" dxfId="0" priority="1995">
+      <formula>IF(ISBLANK($C$1),o,SEARCH($C$1,#REF!&amp;#REF!&amp;#REF!))</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>